<commit_message>
Frontal + cartel ruleta rusa
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 4ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 4ª Version.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hahdm\Workspace\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C04F75-8C2C-4B47-9E5C-0677B12489B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943EEE4D-044D-4B25-A2AB-B5017C14E156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -2157,8 +2157,8 @@
   </sheetPr>
   <dimension ref="A2:P139"/>
   <sheetViews>
-    <sheetView topLeftCell="B94" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105"/>
+    <sheetView tabSelected="1" topLeftCell="B121" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F138" sqref="F138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2212,7 +2212,7 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>329.13</v>
+        <v>330.63</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
@@ -4651,7 +4651,7 @@
       </c>
       <c r="J130">
         <f>F136+F137+F138+F139</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="K130">
         <f>E136+E138+E137+E139</f>
@@ -4762,8 +4762,10 @@
       <c r="E137" s="13">
         <v>2</v>
       </c>
-      <c r="F137" s="13"/>
-      <c r="G137" s="13"/>
+      <c r="F137" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="G137" s="7"/>
     </row>
     <row r="138" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B138" s="54" t="s">
@@ -4829,7 +4831,7 @@
   </sheetPr>
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+    <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -5797,11 +5799,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6014,27 +6017,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6059,9 +6052,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
AL FINAL VOY A JUGAR A LA RULETA RUSA EN AL VIDA REAL + Excel :)
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 4ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 4ª Version.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hahdm\Workspace\Konguitos_Casino\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7831C0E-5141-4080-840E-68C5C83E4363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCA1FC8-C434-4B83-8E2E-CEB6C238678D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2652" yWindow="0" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -1735,7 +1735,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1847,7 +1847,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1903,7 +1903,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2160,20 +2160,20 @@
   </sheetPr>
   <dimension ref="A2:P139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B91" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K131" sqref="K131"/>
+    <sheetView tabSelected="1" topLeftCell="D124" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K134" sqref="K134"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.54296875" customWidth="1"/>
-    <col min="5" max="5" width="13.6328125" customWidth="1"/>
-    <col min="7" max="7" width="53.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.36328125" customWidth="1"/>
-    <col min="11" max="11" width="35.453125" customWidth="1"/>
-    <col min="12" max="12" width="26.6328125" customWidth="1"/>
-    <col min="16" max="16" width="17.453125" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.5546875" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="53.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.33203125" customWidth="1"/>
+    <col min="11" max="11" width="35.44140625" customWidth="1"/>
+    <col min="12" max="12" width="26.6640625" customWidth="1"/>
+    <col min="16" max="16" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2202,7 +2202,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2211,11 +2211,11 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1">
         <f t="shared" ref="E3:F3" si="0">SUM(E6:E994)</f>
-        <v>285.2</v>
+        <v>291.2</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>341.63</v>
+        <v>354.13</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
@@ -2224,7 +2224,7 @@
         <v>87.5</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="59" t="s">
         <v>8</v>
       </c>
@@ -2238,7 +2238,7 @@
       </c>
       <c r="K4" s="65"/>
     </row>
-    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="63"/>
       <c r="C5" s="64"/>
       <c r="D5" s="64"/>
@@ -2546,7 +2546,7 @@
       <c r="J19" s="80"/>
       <c r="K19" s="69"/>
     </row>
-    <row r="20" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>12</v>
       </c>
@@ -2566,7 +2566,7 @@
       <c r="J20" s="80"/>
       <c r="K20" s="69"/>
     </row>
-    <row r="21" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>9</v>
       </c>
@@ -2584,7 +2584,7 @@
       </c>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>9</v>
       </c>
@@ -2607,7 +2607,7 @@
       <c r="K22" s="81"/>
       <c r="L22" s="81"/>
     </row>
-    <row r="23" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
         <v>16</v>
       </c>
@@ -2625,7 +2625,7 @@
       </c>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>13</v>
       </c>
@@ -2643,7 +2643,7 @@
       </c>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
         <v>16</v>
       </c>
@@ -2661,7 +2661,7 @@
       </c>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>13</v>
       </c>
@@ -2679,7 +2679,7 @@
       </c>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
         <v>16</v>
       </c>
@@ -2697,7 +2697,7 @@
       </c>
       <c r="G27" s="7"/>
     </row>
-    <row r="28" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>13</v>
       </c>
@@ -2715,7 +2715,7 @@
       </c>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
         <v>16</v>
       </c>
@@ -2733,7 +2733,7 @@
       </c>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>13</v>
       </c>
@@ -2751,7 +2751,7 @@
       </c>
       <c r="G30" s="7"/>
     </row>
-    <row r="31" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
         <v>16</v>
       </c>
@@ -2768,7 +2768,7 @@
       <c r="G31" s="7"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
         <v>14</v>
       </c>
@@ -2786,7 +2786,7 @@
       </c>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
         <v>14</v>
       </c>
@@ -2802,7 +2802,7 @@
       </c>
       <c r="G33" s="7"/>
     </row>
-    <row r="34" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
         <v>14</v>
       </c>
@@ -2820,7 +2820,7 @@
       </c>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>14</v>
       </c>
@@ -2838,7 +2838,7 @@
       </c>
       <c r="G35" s="7"/>
     </row>
-    <row r="36" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B36" s="8" t="s">
         <v>14</v>
       </c>
@@ -2856,7 +2856,7 @@
       </c>
       <c r="G36" s="7"/>
     </row>
-    <row r="37" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
         <v>14</v>
       </c>
@@ -2874,7 +2874,7 @@
       </c>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
         <v>14</v>
       </c>
@@ -2892,7 +2892,7 @@
       </c>
       <c r="G38" s="7"/>
     </row>
-    <row r="39" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B39" s="9" t="s">
         <v>15</v>
       </c>
@@ -2910,7 +2910,7 @@
       </c>
       <c r="G39" s="7"/>
     </row>
-    <row r="40" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B40" s="9" t="s">
         <v>15</v>
       </c>
@@ -2928,7 +2928,7 @@
       </c>
       <c r="G40" s="7"/>
     </row>
-    <row r="41" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B41" s="59" t="s">
         <v>36</v>
       </c>
@@ -2938,7 +2938,7 @@
       <c r="F41" s="60"/>
       <c r="G41" s="60"/>
     </row>
-    <row r="42" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B42" s="63"/>
       <c r="C42" s="64"/>
       <c r="D42" s="64"/>
@@ -2946,7 +2946,7 @@
       <c r="F42" s="64"/>
       <c r="G42" s="64"/>
     </row>
-    <row r="43" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>12</v>
       </c>
@@ -2964,7 +2964,7 @@
       </c>
       <c r="G43" s="7"/>
     </row>
-    <row r="44" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>13</v>
       </c>
@@ -2982,7 +2982,7 @@
       </c>
       <c r="G44" s="7"/>
     </row>
-    <row r="45" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>12</v>
       </c>
@@ -3000,7 +3000,7 @@
       </c>
       <c r="G45" s="7"/>
     </row>
-    <row r="46" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>12</v>
       </c>
@@ -3018,7 +3018,7 @@
       </c>
       <c r="G46" s="7"/>
     </row>
-    <row r="47" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>12</v>
       </c>
@@ -3036,7 +3036,7 @@
       </c>
       <c r="G47" s="7"/>
     </row>
-    <row r="48" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B48" s="8" t="s">
         <v>14</v>
       </c>
@@ -3054,7 +3054,7 @@
       </c>
       <c r="G48" s="11"/>
     </row>
-    <row r="49" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B49" s="9" t="s">
         <v>15</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
         <v>15</v>
       </c>
@@ -3110,7 +3110,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B51" s="9" t="s">
         <v>15</v>
       </c>
@@ -3139,7 +3139,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>9</v>
       </c>
@@ -3168,7 +3168,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
         <v>9</v>
       </c>
@@ -3197,7 +3197,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>9</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B55" s="6" t="s">
         <v>13</v>
       </c>
@@ -3253,7 +3253,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="56" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B56" s="6" t="s">
         <v>13</v>
       </c>
@@ -3271,7 +3271,7 @@
       </c>
       <c r="G56" s="11"/>
     </row>
-    <row r="57" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B57" s="10" t="s">
         <v>16</v>
       </c>
@@ -3289,7 +3289,7 @@
       </c>
       <c r="G57" s="7"/>
     </row>
-    <row r="58" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B58" s="10" t="s">
         <v>16</v>
       </c>
@@ -3316,7 +3316,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B59" s="10" t="s">
         <v>16</v>
       </c>
@@ -3345,7 +3345,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="60" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B60" s="10" t="s">
         <v>16</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B61" s="6" t="s">
         <v>13</v>
       </c>
@@ -3892,7 +3892,7 @@
       <c r="F84" s="34"/>
       <c r="G84" s="34"/>
     </row>
-    <row r="85" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B85" s="8" t="s">
         <v>14</v>
       </c>
@@ -4046,7 +4046,7 @@
       </c>
       <c r="G93" s="7"/>
     </row>
-    <row r="94" spans="2:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:7" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="4" t="s">
         <v>9</v>
       </c>
@@ -4711,11 +4711,23 @@
         <v>161</v>
       </c>
       <c r="D133" s="13"/>
-      <c r="E133" s="13"/>
-      <c r="F133" s="13"/>
+      <c r="E133" s="13">
+        <v>6</v>
+      </c>
+      <c r="F133" s="13">
+        <v>12.5</v>
+      </c>
       <c r="G133" s="13"/>
       <c r="I133" s="5" t="s">
         <v>12</v>
+      </c>
+      <c r="J133">
+        <f>F133</f>
+        <v>12.5</v>
+      </c>
+      <c r="K133">
+        <f>E133</f>
+        <v>6</v>
       </c>
     </row>
     <row r="134" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4856,13 +4868,13 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.54296875" customWidth="1"/>
-    <col min="2" max="2" width="35.453125" customWidth="1"/>
-    <col min="3" max="3" width="27.36328125" customWidth="1"/>
-    <col min="4" max="4" width="10.36328125" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4925,7 +4937,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -4948,7 +4960,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -5190,7 +5202,7 @@
       <c r="F17" s="13"/>
       <c r="G17" s="15"/>
     </row>
-    <row r="18" spans="1:7" ht="14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>17</v>
       </c>
@@ -5213,7 +5225,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>18</v>
       </c>
@@ -5236,7 +5248,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>19</v>
       </c>
@@ -5250,7 +5262,7 @@
       <c r="F20" s="13"/>
       <c r="G20" s="15"/>
     </row>
-    <row r="21" spans="1:7" ht="14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>20</v>
       </c>
@@ -5271,7 +5283,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>21</v>
       </c>
@@ -5286,7 +5298,7 @@
       <c r="F22" s="13"/>
       <c r="G22" s="15"/>
     </row>
-    <row r="23" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>22</v>
       </c>
@@ -5301,7 +5313,7 @@
       <c r="F23" s="13"/>
       <c r="G23" s="15"/>
     </row>
-    <row r="24" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>23</v>
       </c>
@@ -5322,7 +5334,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>24</v>
       </c>
@@ -5337,7 +5349,7 @@
       <c r="F25" s="13"/>
       <c r="G25" s="15"/>
     </row>
-    <row r="26" spans="1:7" ht="14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>25</v>
       </c>
@@ -5360,7 +5372,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>26</v>
       </c>
@@ -5375,7 +5387,7 @@
       <c r="F27" s="13"/>
       <c r="G27" s="15"/>
     </row>
-    <row r="28" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>27</v>
       </c>
@@ -5398,7 +5410,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>28</v>
       </c>
@@ -5413,7 +5425,7 @@
       <c r="F29" s="13"/>
       <c r="G29" s="15"/>
     </row>
-    <row r="30" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>29</v>
       </c>
@@ -5428,7 +5440,7 @@
       <c r="F30" s="13"/>
       <c r="G30" s="15"/>
     </row>
-    <row r="31" spans="1:7" ht="14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <v>30</v>
       </c>
@@ -5451,7 +5463,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <v>31</v>
       </c>
@@ -5472,7 +5484,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <v>32</v>
       </c>
@@ -5493,7 +5505,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <v>33</v>
       </c>
@@ -5514,7 +5526,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>34</v>
       </c>
@@ -5531,7 +5543,7 @@
       <c r="F35" s="13"/>
       <c r="G35" s="15"/>
     </row>
-    <row r="36" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>35</v>
       </c>
@@ -5546,7 +5558,7 @@
       <c r="F36" s="13"/>
       <c r="G36" s="15"/>
     </row>
-    <row r="37" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>36</v>
       </c>
@@ -5569,7 +5581,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <v>37</v>
       </c>
@@ -5586,7 +5598,7 @@
       <c r="F38" s="13"/>
       <c r="G38" s="15"/>
     </row>
-    <row r="39" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <v>38</v>
       </c>
@@ -5601,7 +5613,7 @@
       <c r="F39" s="13"/>
       <c r="G39" s="15"/>
     </row>
-    <row r="40" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <v>39</v>
       </c>
@@ -5622,7 +5634,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <v>40</v>
       </c>
@@ -5645,7 +5657,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <v>41</v>
       </c>
@@ -5668,7 +5680,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <v>42</v>
       </c>
@@ -5691,7 +5703,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <v>43</v>
       </c>
@@ -5714,7 +5726,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <v>44</v>
       </c>
@@ -5735,7 +5747,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <v>45</v>
       </c>
@@ -5750,7 +5762,7 @@
       <c r="F46" s="13"/>
       <c r="G46" s="15"/>
     </row>
-    <row r="47" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <v>46</v>
       </c>
@@ -5820,12 +5832,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6038,17 +6049,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6073,18 +6094,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
refactorizando y arreglando errores y las ganas de suicidarse
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 4ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 4ª Version.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34616\Desktop\CEU\tercer año\primer_semestre\ing_software\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C232838-ABCE-426F-8E28-F6641CAE924B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D510817-E8B0-43DF-9DFF-55017F6FB601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="630" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="185">
   <si>
     <t>Nombre</t>
   </si>
@@ -615,6 +615,12 @@
   </si>
   <si>
     <t>Interfaz ventana principal</t>
+  </si>
+  <si>
+    <t>bajo demanda</t>
+  </si>
+  <si>
+    <t>apoyo toolbar</t>
   </si>
 </sst>
 </file>
@@ -1732,7 +1738,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1844,7 +1850,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1900,7 +1906,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2155,10 +2161,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:P139"/>
+  <dimension ref="A2:P140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B94" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J139" sqref="J139"/>
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K145" sqref="K145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2208,17 +2214,17 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1">
         <f t="shared" ref="E3:F3" si="0">SUM(E6:E995)</f>
-        <v>289.2</v>
+        <v>292.2</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>331.13</v>
+        <v>358.29</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
       <c r="K3" s="65">
-        <f>F6+F12+F22+F21+F52+F53+F54+F62+F63+F64+F65+F71+J73</f>
-        <v>87.5</v>
+        <f>F6+F12+F22+F21+F52+F53+F54+F62+F63+F64+F65+F71+J73+J130</f>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2267,8 +2273,8 @@
         <v>12</v>
       </c>
       <c r="K6" s="69">
-        <f>F7+F13+F20+F43+F45+F47+F46+J76+F75+F89+F90+F99+F100+F115+F116+F117</f>
-        <v>62.7</v>
+        <f>F7+F13+F20+F43+F45+F47+F46+J76+F75+F89+F90+F99+F100+F115+F116+F117+J133</f>
+        <v>75.2</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -2335,8 +2341,8 @@
         <v>13</v>
       </c>
       <c r="K9" s="69">
-        <f>F8+F14+F19+F24+F26+F28+F30+F44+F55+F56+F61+F66+J74</f>
-        <v>80.930000000000007</v>
+        <f>F8+F14+F19+F24+F26+F28+F30+F44+F55+F56+F61+F66+J74+J131</f>
+        <v>86.59</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -3672,7 +3678,7 @@
       </c>
       <c r="J74">
         <f>F80+F91+F102+F104+F103+F118+F119+F120</f>
-        <v>35.21</v>
+        <v>36.870000000000005</v>
       </c>
       <c r="K74">
         <f>E80+E91+E102+E103+E104+E118+E119+E120</f>
@@ -3823,7 +3829,7 @@
       <c r="F80" s="34">
         <v>9</v>
       </c>
-      <c r="G80" s="11"/>
+      <c r="G80" s="49"/>
     </row>
     <row r="81" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="10" t="s">
@@ -4003,7 +4009,7 @@
         <v>6</v>
       </c>
       <c r="F91" s="34">
-        <v>4.2</v>
+        <v>5.7</v>
       </c>
       <c r="G91" s="11"/>
     </row>
@@ -4211,7 +4217,7 @@
         <v>2</v>
       </c>
       <c r="F103" s="1">
-        <v>4.34</v>
+        <v>4.5</v>
       </c>
       <c r="G103" s="11"/>
     </row>
@@ -4471,7 +4477,7 @@
       <c r="F118" s="34">
         <v>12</v>
       </c>
-      <c r="G118" s="11"/>
+      <c r="G118" s="7"/>
     </row>
     <row r="119" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B119" s="45" t="s">
@@ -4643,15 +4649,19 @@
         <v>178</v>
       </c>
       <c r="D130" s="13"/>
-      <c r="E130" s="13"/>
-      <c r="F130" s="13"/>
+      <c r="E130" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="F130" s="13">
+        <v>1.5</v>
+      </c>
       <c r="G130" s="13"/>
       <c r="I130" s="57" t="s">
         <v>9</v>
       </c>
       <c r="J130">
         <f>F136+F137+F138+F139</f>
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="K130">
         <f>E136+E138+E137+E139</f>
@@ -4667,22 +4677,22 @@
       </c>
       <c r="D131" s="13"/>
       <c r="E131" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F131" s="13">
-        <v>2</v>
-      </c>
-      <c r="G131" s="11"/>
+        <v>2.5</v>
+      </c>
+      <c r="G131" s="7"/>
       <c r="I131" s="6" t="s">
         <v>13</v>
       </c>
       <c r="J131">
         <f>F131+F130</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K131">
         <f>E131</f>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="132" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4708,11 +4718,23 @@
         <v>161</v>
       </c>
       <c r="D133" s="13"/>
-      <c r="E133" s="13"/>
-      <c r="F133" s="13"/>
-      <c r="G133" s="13"/>
+      <c r="E133" s="13">
+        <v>6</v>
+      </c>
+      <c r="F133" s="13">
+        <v>12.5</v>
+      </c>
+      <c r="G133" s="11"/>
       <c r="I133" s="5" t="s">
         <v>12</v>
+      </c>
+      <c r="J133">
+        <f>F133</f>
+        <v>12.5</v>
+      </c>
+      <c r="K133">
+        <f>E133</f>
+        <v>6</v>
       </c>
     </row>
     <row r="134" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4774,8 +4796,10 @@
       <c r="E137" s="13">
         <v>2</v>
       </c>
-      <c r="F137" s="13"/>
-      <c r="G137" s="13"/>
+      <c r="F137" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="G137" s="7"/>
     </row>
     <row r="138" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B138" s="54" t="s">
@@ -4790,8 +4814,10 @@
       <c r="E138" s="13">
         <v>4</v>
       </c>
-      <c r="F138" s="13"/>
-      <c r="G138" s="13"/>
+      <c r="F138" s="13">
+        <v>6</v>
+      </c>
+      <c r="G138" s="11"/>
     </row>
     <row r="139" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B139" s="54" t="s">
@@ -4806,8 +4832,26 @@
       <c r="E139" s="13">
         <v>4</v>
       </c>
-      <c r="F139" s="13"/>
-      <c r="G139" s="13"/>
+      <c r="F139" s="13">
+        <v>3</v>
+      </c>
+      <c r="G139" s="7"/>
+    </row>
+    <row r="140" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B140" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="C140" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="D140" s="13"/>
+      <c r="E140" s="13">
+        <v>0</v>
+      </c>
+      <c r="F140" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G140" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -4829,8 +4873,9 @@
     <mergeCell ref="J22:L22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Actualización Horas y Ruleta: Apuestas(1.0) y Alertas
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 4ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 4ª Version.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hahdm\Workspace\Konguitos_Casino\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanzc\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64C8893-AC39-40DA-9B3B-04351F64568A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D505BC85-EAC1-4ABC-BAE1-2AA31C93B34B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29940" yWindow="1140" windowWidth="21600" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -1236,7 +1236,7 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>16770</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>15758</xdr:rowOff>
+      <xdr:rowOff>12583</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1541,7 +1541,7 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>15801</xdr:rowOff>
+      <xdr:rowOff>12626</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2188,8 +2188,8 @@
   </sheetPr>
   <dimension ref="A2:P140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B119" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F139" sqref="F139"/>
+    <sheetView tabSelected="1" topLeftCell="B123" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I137" sqref="I137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2239,7 +2239,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1">
         <f t="shared" ref="E3:F3" si="0">SUM(E6:E995)</f>
-        <v>305.2</v>
+        <v>308.2</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
@@ -2430,7 +2430,7 @@
       </c>
       <c r="K12" s="69">
         <f>F9+F15+F32+F33+F34+F35+F36+F37+F38+F48+F67+F68+J77+J134</f>
-        <v>57.85</v>
+        <v>60.85</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4771,7 +4771,7 @@
       </c>
       <c r="D134" s="13"/>
       <c r="E134" s="13">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F134" s="13"/>
       <c r="G134" s="13"/>
@@ -4780,7 +4780,7 @@
       </c>
       <c r="J134" cm="1">
         <f t="array" ref="J134:J135">E134:E135</f>
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="135" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5897,14 +5897,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002ACE3BD3BD6E0C4C9762278BB0DF607B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fab7ba1af23be20b30c2a2672ed67a22">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf" xmlns:ns4="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="531abb56a789977dee09b3cb67363cc8" ns3:_="" ns4:_="">
     <xsd:import namespace="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
@@ -6113,6 +6105,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
   <ds:schemaRefs>
@@ -6122,23 +6122,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6155,4 +6138,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Mis horas para que Hugo no me coma
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 4ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 4ª Version.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34616\Desktop\CEU\tercer año\primer_semestre\ing_software\Konguitos_Casino\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7nume\OneDrive\Documentos\CEU\3- Tercero\Software\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45D7C32-2B31-4D3A-94A1-9BB97BA886B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9182325E-B3BE-43AC-B600-22322A8CC6FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="186">
   <si>
     <t>Nombre</t>
   </si>
@@ -2186,10 +2186,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:P140"/>
+  <dimension ref="A2:P141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B68" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F131" sqref="F131"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2238,12 +2238,12 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:F3" si="0">SUM(E6:E995)</f>
-        <v>305.2</v>
+        <f t="shared" ref="E3:F3" si="0">SUM(E6:E996)</f>
+        <v>307.2</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>360.46000000000004</v>
+        <v>365.96000000000004</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
@@ -2488,8 +2488,8 @@
         <v>15</v>
       </c>
       <c r="K15" s="69">
-        <f>F10+F16+F39+F40+F49+F50+F51+J75</f>
-        <v>36.5</v>
+        <f>F10+F16+F39+F40+F49+F50+F51+J75+J132</f>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4653,9 +4653,13 @@
         <v>177</v>
       </c>
       <c r="D129" s="13"/>
-      <c r="E129" s="13"/>
-      <c r="F129" s="13"/>
-      <c r="G129" s="13"/>
+      <c r="E129" s="13">
+        <v>1</v>
+      </c>
+      <c r="F129" s="13">
+        <v>2</v>
+      </c>
+      <c r="G129" s="11"/>
       <c r="I129" s="58" t="s">
         <v>185</v>
       </c>
@@ -4667,29 +4671,29 @@
       </c>
     </row>
     <row r="130" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B130" s="52" t="s">
-        <v>13</v>
+      <c r="B130" s="51" t="s">
+        <v>15</v>
       </c>
       <c r="C130" s="13" t="s">
-        <v>178</v>
+        <v>71</v>
       </c>
       <c r="D130" s="13"/>
-      <c r="E130" s="13" t="s">
-        <v>183</v>
+      <c r="E130" s="13">
+        <v>1</v>
       </c>
       <c r="F130" s="13">
-        <v>3.67</v>
-      </c>
-      <c r="G130" s="11"/>
+        <v>3.5</v>
+      </c>
+      <c r="G130" s="7"/>
       <c r="I130" s="57" t="s">
         <v>9</v>
       </c>
       <c r="J130">
-        <f>F136+F137+F138+F139</f>
+        <f>F137+F138+F139+F140</f>
         <v>10.5</v>
       </c>
       <c r="K130">
-        <f>E136+E138+E137+E139</f>
+        <f>E137+E139+E138+E140</f>
         <v>30</v>
       </c>
     </row>
@@ -4698,88 +4702,98 @@
         <v>13</v>
       </c>
       <c r="C131" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D131" s="13"/>
-      <c r="E131" s="13">
-        <v>2</v>
+      <c r="E131" s="13" t="s">
+        <v>183</v>
       </c>
       <c r="F131" s="13">
-        <v>2.5</v>
-      </c>
-      <c r="G131" s="7"/>
+        <v>3.67</v>
+      </c>
+      <c r="G131" s="11"/>
       <c r="I131" s="6" t="s">
         <v>13</v>
       </c>
       <c r="J131">
-        <f>F131+F130</f>
+        <f>F132+F131</f>
         <v>6.17</v>
       </c>
       <c r="K131">
-        <f>E131</f>
+        <f>E132</f>
         <v>2</v>
       </c>
     </row>
     <row r="132" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B132" s="53" t="s">
-        <v>16</v>
+      <c r="B132" s="52" t="s">
+        <v>13</v>
       </c>
       <c r="C132" s="13" t="s">
-        <v>125</v>
+        <v>179</v>
       </c>
       <c r="D132" s="13"/>
-      <c r="E132" s="13"/>
-      <c r="F132" s="13"/>
-      <c r="G132" s="13"/>
+      <c r="E132" s="13">
+        <v>2</v>
+      </c>
+      <c r="F132" s="13">
+        <v>2.5</v>
+      </c>
+      <c r="G132" s="7"/>
       <c r="I132" s="9" t="s">
         <v>15</v>
       </c>
+      <c r="J132">
+        <f>F130+F129</f>
+        <v>5.5</v>
+      </c>
+      <c r="K132">
+        <f>E129+E130</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="133" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B133" s="55" t="s">
-        <v>12</v>
+      <c r="B133" s="53" t="s">
+        <v>16</v>
       </c>
       <c r="C133" s="13" t="s">
-        <v>161</v>
+        <v>125</v>
       </c>
       <c r="D133" s="13"/>
-      <c r="E133" s="13">
-        <v>6</v>
-      </c>
-      <c r="F133" s="13">
-        <v>12.5</v>
-      </c>
-      <c r="G133" s="11"/>
+      <c r="E133" s="13"/>
+      <c r="F133" s="13"/>
+      <c r="G133" s="13"/>
       <c r="I133" s="5" t="s">
         <v>12</v>
       </c>
       <c r="J133">
-        <f>F133</f>
+        <f>F134</f>
         <v>12.5</v>
       </c>
       <c r="K133">
-        <f>E133</f>
+        <f>E134</f>
         <v>6</v>
       </c>
     </row>
     <row r="134" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B134" s="56" t="s">
-        <v>14</v>
+      <c r="B134" s="55" t="s">
+        <v>12</v>
       </c>
       <c r="C134" s="13" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="D134" s="13"/>
       <c r="E134" s="13">
-        <v>13</v>
-      </c>
-      <c r="F134" s="13"/>
-      <c r="G134" s="13"/>
+        <v>6</v>
+      </c>
+      <c r="F134" s="13">
+        <v>12.5</v>
+      </c>
+      <c r="G134" s="11"/>
       <c r="I134" s="8" t="s">
         <v>14</v>
       </c>
       <c r="J134" cm="1">
-        <f t="array" ref="J134:J135">E134:E135</f>
+        <f t="array" ref="J134:J135">E135:E136</f>
         <v>13</v>
       </c>
     </row>
@@ -4788,10 +4802,12 @@
         <v>14</v>
       </c>
       <c r="C135" s="13" t="s">
-        <v>82</v>
+        <v>180</v>
       </c>
       <c r="D135" s="13"/>
-      <c r="E135" s="13"/>
+      <c r="E135" s="13">
+        <v>13</v>
+      </c>
       <c r="F135" s="13"/>
       <c r="G135" s="13"/>
       <c r="I135" s="10" t="s">
@@ -4802,18 +4818,14 @@
       </c>
     </row>
     <row r="136" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B136" s="54" t="s">
-        <v>9</v>
+      <c r="B136" s="56" t="s">
+        <v>14</v>
       </c>
       <c r="C136" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="D136" s="13">
-        <v>24</v>
-      </c>
-      <c r="E136" s="13">
-        <v>20</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="D136" s="13"/>
+      <c r="E136" s="13"/>
       <c r="F136" s="13"/>
       <c r="G136" s="13"/>
     </row>
@@ -4822,43 +4834,41 @@
         <v>9</v>
       </c>
       <c r="C137" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="D137" s="13" t="s">
-        <v>11</v>
+        <v>124</v>
+      </c>
+      <c r="D137" s="13">
+        <v>24</v>
       </c>
       <c r="E137" s="13">
-        <v>2</v>
-      </c>
-      <c r="F137" s="13">
-        <v>1.5</v>
-      </c>
-      <c r="G137" s="7"/>
+        <v>20</v>
+      </c>
+      <c r="F137" s="13"/>
+      <c r="G137" s="13"/>
     </row>
     <row r="138" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B138" s="54" t="s">
         <v>9</v>
       </c>
       <c r="C138" s="13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D138" s="13" t="s">
         <v>11</v>
       </c>
       <c r="E138" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F138" s="13">
-        <v>6</v>
-      </c>
-      <c r="G138" s="11"/>
+        <v>1.5</v>
+      </c>
+      <c r="G138" s="7"/>
     </row>
     <row r="139" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B139" s="54" t="s">
         <v>9</v>
       </c>
       <c r="C139" s="13" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="D139" s="13" t="s">
         <v>11</v>
@@ -4867,25 +4877,43 @@
         <v>4</v>
       </c>
       <c r="F139" s="13">
+        <v>6</v>
+      </c>
+      <c r="G139" s="11"/>
+    </row>
+    <row r="140" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B140" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C140" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="D140" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E140" s="13">
+        <v>4</v>
+      </c>
+      <c r="F140" s="13">
         <v>3</v>
       </c>
-      <c r="G139" s="7"/>
-    </row>
-    <row r="140" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B140" s="53" t="s">
+      <c r="G140" s="7"/>
+    </row>
+    <row r="141" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B141" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="C140" s="13" t="s">
+      <c r="C141" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="D140" s="13"/>
-      <c r="E140" s="13">
+      <c r="D141" s="13"/>
+      <c r="E141" s="13">
         <v>0</v>
       </c>
-      <c r="F140" s="13">
+      <c r="F141" s="13">
         <v>0.5</v>
       </c>
-      <c r="G140" s="7"/>
+      <c r="G141" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -5897,14 +5925,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002ACE3BD3BD6E0C4C9762278BB0DF607B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fab7ba1af23be20b30c2a2672ed67a22">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf" xmlns:ns4="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="531abb56a789977dee09b3cb67363cc8" ns3:_="" ns4:_="">
     <xsd:import namespace="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
@@ -6113,6 +6133,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
   <ds:schemaRefs>
@@ -6122,23 +6150,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6155,4 +6166,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Hugu y sus 100 horas
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 4ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 4ª Version.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7nume\OneDrive\Documentos\CEU\3- Tercero\Software\Konguitos_Casino\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hahdm\Workspace\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9182325E-B3BE-43AC-B600-22322A8CC6FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B659DF-8610-490A-8D2D-9A0605FA3827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -2188,20 +2188,20 @@
   </sheetPr>
   <dimension ref="A2:P141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="B118" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F138" sqref="F138"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="7" max="7" width="53.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.33203125" customWidth="1"/>
-    <col min="11" max="11" width="35.44140625" customWidth="1"/>
-    <col min="12" max="12" width="26.6640625" customWidth="1"/>
-    <col min="16" max="16" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="5.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.6328125" customWidth="1"/>
+    <col min="7" max="7" width="53.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.36328125" customWidth="1"/>
+    <col min="11" max="11" width="35.453125" customWidth="1"/>
+    <col min="12" max="12" width="26.6328125" customWidth="1"/>
+    <col min="16" max="16" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2230,7 +2230,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2243,16 +2243,16 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>365.96000000000004</v>
+        <v>370.96000000000004</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
       <c r="K3" s="65">
         <f>F6+F12+F22+F21+F52+F53+F54+F62+F63+F64+F65+F71+J73+J130</f>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="59" t="s">
         <v>8</v>
       </c>
@@ -2266,7 +2266,7 @@
       </c>
       <c r="K4" s="65"/>
     </row>
-    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="63"/>
       <c r="C5" s="64"/>
       <c r="D5" s="64"/>
@@ -2574,7 +2574,7 @@
       <c r="J19" s="80"/>
       <c r="K19" s="69"/>
     </row>
-    <row r="20" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>12</v>
       </c>
@@ -2594,7 +2594,7 @@
       <c r="J20" s="80"/>
       <c r="K20" s="69"/>
     </row>
-    <row r="21" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>9</v>
       </c>
@@ -2612,7 +2612,7 @@
       </c>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>9</v>
       </c>
@@ -2635,7 +2635,7 @@
       <c r="K22" s="81"/>
       <c r="L22" s="81"/>
     </row>
-    <row r="23" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
         <v>16</v>
       </c>
@@ -2653,7 +2653,7 @@
       </c>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>13</v>
       </c>
@@ -2671,7 +2671,7 @@
       </c>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
         <v>16</v>
       </c>
@@ -2689,7 +2689,7 @@
       </c>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>13</v>
       </c>
@@ -2707,7 +2707,7 @@
       </c>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
         <v>16</v>
       </c>
@@ -2725,7 +2725,7 @@
       </c>
       <c r="G27" s="7"/>
     </row>
-    <row r="28" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>13</v>
       </c>
@@ -2743,7 +2743,7 @@
       </c>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
         <v>16</v>
       </c>
@@ -2761,7 +2761,7 @@
       </c>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>13</v>
       </c>
@@ -2779,7 +2779,7 @@
       </c>
       <c r="G30" s="7"/>
     </row>
-    <row r="31" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
         <v>16</v>
       </c>
@@ -2796,7 +2796,7 @@
       <c r="G31" s="7"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
         <v>14</v>
       </c>
@@ -2814,7 +2814,7 @@
       </c>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
         <v>14</v>
       </c>
@@ -2830,7 +2830,7 @@
       </c>
       <c r="G33" s="7"/>
     </row>
-    <row r="34" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
         <v>14</v>
       </c>
@@ -2848,7 +2848,7 @@
       </c>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>14</v>
       </c>
@@ -2866,7 +2866,7 @@
       </c>
       <c r="G35" s="7"/>
     </row>
-    <row r="36" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B36" s="8" t="s">
         <v>14</v>
       </c>
@@ -2884,7 +2884,7 @@
       </c>
       <c r="G36" s="7"/>
     </row>
-    <row r="37" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
         <v>14</v>
       </c>
@@ -2902,7 +2902,7 @@
       </c>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
         <v>14</v>
       </c>
@@ -2920,7 +2920,7 @@
       </c>
       <c r="G38" s="7"/>
     </row>
-    <row r="39" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B39" s="9" t="s">
         <v>15</v>
       </c>
@@ -2938,7 +2938,7 @@
       </c>
       <c r="G39" s="7"/>
     </row>
-    <row r="40" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B40" s="9" t="s">
         <v>15</v>
       </c>
@@ -2956,7 +2956,7 @@
       </c>
       <c r="G40" s="7"/>
     </row>
-    <row r="41" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B41" s="59" t="s">
         <v>36</v>
       </c>
@@ -2966,7 +2966,7 @@
       <c r="F41" s="60"/>
       <c r="G41" s="60"/>
     </row>
-    <row r="42" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B42" s="63"/>
       <c r="C42" s="64"/>
       <c r="D42" s="64"/>
@@ -2974,7 +2974,7 @@
       <c r="F42" s="64"/>
       <c r="G42" s="64"/>
     </row>
-    <row r="43" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>12</v>
       </c>
@@ -2992,7 +2992,7 @@
       </c>
       <c r="G43" s="7"/>
     </row>
-    <row r="44" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>13</v>
       </c>
@@ -3010,7 +3010,7 @@
       </c>
       <c r="G44" s="7"/>
     </row>
-    <row r="45" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>12</v>
       </c>
@@ -3028,7 +3028,7 @@
       </c>
       <c r="G45" s="7"/>
     </row>
-    <row r="46" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>12</v>
       </c>
@@ -3046,7 +3046,7 @@
       </c>
       <c r="G46" s="7"/>
     </row>
-    <row r="47" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>12</v>
       </c>
@@ -3064,7 +3064,7 @@
       </c>
       <c r="G47" s="7"/>
     </row>
-    <row r="48" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B48" s="8" t="s">
         <v>14</v>
       </c>
@@ -3082,7 +3082,7 @@
       </c>
       <c r="G48" s="11"/>
     </row>
-    <row r="49" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B49" s="9" t="s">
         <v>15</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
         <v>15</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B51" s="9" t="s">
         <v>15</v>
       </c>
@@ -3167,7 +3167,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>9</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
         <v>9</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>9</v>
       </c>
@@ -3254,7 +3254,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B55" s="6" t="s">
         <v>13</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="56" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B56" s="6" t="s">
         <v>13</v>
       </c>
@@ -3299,7 +3299,7 @@
       </c>
       <c r="G56" s="11"/>
     </row>
-    <row r="57" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B57" s="10" t="s">
         <v>16</v>
       </c>
@@ -3317,7 +3317,7 @@
       </c>
       <c r="G57" s="7"/>
     </row>
-    <row r="58" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B58" s="10" t="s">
         <v>16</v>
       </c>
@@ -3344,7 +3344,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B59" s="10" t="s">
         <v>16</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="60" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B60" s="10" t="s">
         <v>16</v>
       </c>
@@ -3402,7 +3402,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B61" s="6" t="s">
         <v>13</v>
       </c>
@@ -3920,7 +3920,7 @@
       <c r="F84" s="34"/>
       <c r="G84" s="34"/>
     </row>
-    <row r="85" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B85" s="8" t="s">
         <v>14</v>
       </c>
@@ -4074,7 +4074,7 @@
       </c>
       <c r="G93" s="7"/>
     </row>
-    <row r="94" spans="2:7" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="4" t="s">
         <v>9</v>
       </c>
@@ -4690,7 +4690,7 @@
       </c>
       <c r="J130">
         <f>F137+F138+F139+F140</f>
-        <v>10.5</v>
+        <v>15.5</v>
       </c>
       <c r="K130">
         <f>E137+E139+E138+E140</f>
@@ -4842,8 +4842,10 @@
       <c r="E137" s="13">
         <v>20</v>
       </c>
-      <c r="F137" s="13"/>
-      <c r="G137" s="13"/>
+      <c r="F137" s="13">
+        <v>4</v>
+      </c>
+      <c r="G137" s="11"/>
     </row>
     <row r="138" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B138" s="54" t="s">
@@ -4877,9 +4879,9 @@
         <v>4</v>
       </c>
       <c r="F139" s="13">
-        <v>6</v>
-      </c>
-      <c r="G139" s="11"/>
+        <v>7</v>
+      </c>
+      <c r="G139" s="7"/>
     </row>
     <row r="140" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B140" s="54" t="s">
@@ -4952,13 +4954,13 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" customWidth="1"/>
+    <col min="2" max="2" width="35.453125" customWidth="1"/>
+    <col min="3" max="3" width="27.36328125" customWidth="1"/>
+    <col min="4" max="4" width="10.36328125" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5021,7 +5023,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -5044,7 +5046,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -5286,7 +5288,7 @@
       <c r="F17" s="13"/>
       <c r="G17" s="15"/>
     </row>
-    <row r="18" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A18" s="15">
         <v>17</v>
       </c>
@@ -5309,7 +5311,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A19" s="15">
         <v>18</v>
       </c>
@@ -5332,7 +5334,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>19</v>
       </c>
@@ -5346,7 +5348,7 @@
       <c r="F20" s="13"/>
       <c r="G20" s="15"/>
     </row>
-    <row r="21" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A21" s="15">
         <v>20</v>
       </c>
@@ -5367,7 +5369,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>21</v>
       </c>
@@ -5382,7 +5384,7 @@
       <c r="F22" s="13"/>
       <c r="G22" s="15"/>
     </row>
-    <row r="23" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>22</v>
       </c>
@@ -5397,7 +5399,7 @@
       <c r="F23" s="13"/>
       <c r="G23" s="15"/>
     </row>
-    <row r="24" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>23</v>
       </c>
@@ -5418,7 +5420,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>24</v>
       </c>
@@ -5433,7 +5435,7 @@
       <c r="F25" s="13"/>
       <c r="G25" s="15"/>
     </row>
-    <row r="26" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A26" s="15">
         <v>25</v>
       </c>
@@ -5456,7 +5458,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>26</v>
       </c>
@@ -5471,7 +5473,7 @@
       <c r="F27" s="13"/>
       <c r="G27" s="15"/>
     </row>
-    <row r="28" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>27</v>
       </c>
@@ -5494,7 +5496,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>28</v>
       </c>
@@ -5509,7 +5511,7 @@
       <c r="F29" s="13"/>
       <c r="G29" s="15"/>
     </row>
-    <row r="30" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>29</v>
       </c>
@@ -5524,7 +5526,7 @@
       <c r="F30" s="13"/>
       <c r="G30" s="15"/>
     </row>
-    <row r="31" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A31" s="15">
         <v>30</v>
       </c>
@@ -5547,7 +5549,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A32" s="15">
         <v>31</v>
       </c>
@@ -5568,7 +5570,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A33" s="15">
         <v>32</v>
       </c>
@@ -5589,7 +5591,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A34" s="15">
         <v>33</v>
       </c>
@@ -5610,7 +5612,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>34</v>
       </c>
@@ -5627,7 +5629,7 @@
       <c r="F35" s="13"/>
       <c r="G35" s="15"/>
     </row>
-    <row r="36" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>35</v>
       </c>
@@ -5642,7 +5644,7 @@
       <c r="F36" s="13"/>
       <c r="G36" s="15"/>
     </row>
-    <row r="37" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>36</v>
       </c>
@@ -5665,7 +5667,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <v>37</v>
       </c>
@@ -5682,7 +5684,7 @@
       <c r="F38" s="13"/>
       <c r="G38" s="15"/>
     </row>
-    <row r="39" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <v>38</v>
       </c>
@@ -5697,7 +5699,7 @@
       <c r="F39" s="13"/>
       <c r="G39" s="15"/>
     </row>
-    <row r="40" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <v>39</v>
       </c>
@@ -5718,7 +5720,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <v>40</v>
       </c>
@@ -5741,7 +5743,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <v>41</v>
       </c>
@@ -5764,7 +5766,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <v>42</v>
       </c>
@@ -5787,7 +5789,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A44" s="15">
         <v>43</v>
       </c>
@@ -5810,7 +5812,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <v>44</v>
       </c>
@@ -5831,7 +5833,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <v>45</v>
       </c>
@@ -5846,7 +5848,7 @@
       <c r="F46" s="13"/>
       <c r="G46" s="15"/>
     </row>
-    <row r="47" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <v>46</v>
       </c>
@@ -5925,6 +5927,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002ACE3BD3BD6E0C4C9762278BB0DF607B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fab7ba1af23be20b30c2a2672ed67a22">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf" xmlns:ns4="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="531abb56a789977dee09b3cb67363cc8" ns3:_="" ns4:_="">
     <xsd:import namespace="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
@@ -6133,14 +6143,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
   <ds:schemaRefs>
@@ -6150,6 +6152,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6166,21 +6185,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Excel arreglado a horas totales
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 4ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 4ª Version.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hahdm\Workspace\Konguitos_Casino\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BAEF17-F9FF-400D-8450-AA093F1ADFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01942908-3111-4E66-BDC4-29A6A4CDBB02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -2169,20 +2169,20 @@
   </sheetPr>
   <dimension ref="A2:P141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="60" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B140" sqref="B140:G140"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="60" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3:K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.54296875" customWidth="1"/>
-    <col min="5" max="5" width="13.6328125" customWidth="1"/>
-    <col min="7" max="7" width="53.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.36328125" customWidth="1"/>
-    <col min="11" max="11" width="35.453125" customWidth="1"/>
-    <col min="12" max="12" width="26.6328125" customWidth="1"/>
-    <col min="16" max="16" width="17.453125" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.5546875" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="53.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.33203125" customWidth="1"/>
+    <col min="11" max="11" width="35.44140625" customWidth="1"/>
+    <col min="12" max="12" width="26.6640625" customWidth="1"/>
+    <col min="16" max="16" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2211,7 +2211,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2220,11 +2220,11 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1">
         <f t="shared" ref="E3:F3" si="0">SUM(E6:E996)</f>
-        <v>306.2</v>
+        <v>298.2</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>378.46000000000004</v>
+        <v>401.36</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
@@ -2233,7 +2233,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="59" t="s">
         <v>8</v>
       </c>
@@ -2247,7 +2247,7 @@
       </c>
       <c r="K4" s="65"/>
     </row>
-    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="63"/>
       <c r="C5" s="64"/>
       <c r="D5" s="64"/>
@@ -2279,8 +2279,8 @@
         <v>12</v>
       </c>
       <c r="K6" s="69">
-        <f>F7+F13+F20+F43+F45+F47+F46+J76+F75+F89+F90+F99+F100+F115+F116+F117+J133</f>
-        <v>75.2</v>
+        <f>F7+F13+F20+F43+F45+F47+F46+J76+J133</f>
+        <v>64.5</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -2411,7 +2411,7 @@
       </c>
       <c r="K12" s="69">
         <f>F9+F15+F32+F33+F34+F35+F36+F37+F38+F48+F67+F68+J77+J134</f>
-        <v>60.85</v>
+        <v>62.85</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2530,8 +2530,8 @@
         <v>16</v>
       </c>
       <c r="K18" s="69">
-        <f>F11+F23+F25+F27+F29+F31+F57+F58+F59+F60+F69+F70+F79+F82+F81+J78</f>
-        <v>35.75</v>
+        <f>F11+F23+F25+F27+F29+F31+F57+F58+F59+F60+F69+F70+J78+J135</f>
+        <v>36.75</v>
       </c>
     </row>
     <row r="19" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2555,7 +2555,7 @@
       <c r="J19" s="80"/>
       <c r="K19" s="69"/>
     </row>
-    <row r="20" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>12</v>
       </c>
@@ -2575,7 +2575,7 @@
       <c r="J20" s="80"/>
       <c r="K20" s="69"/>
     </row>
-    <row r="21" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>9</v>
       </c>
@@ -2593,7 +2593,7 @@
       </c>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>9</v>
       </c>
@@ -2616,7 +2616,7 @@
       <c r="K22" s="81"/>
       <c r="L22" s="81"/>
     </row>
-    <row r="23" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
         <v>16</v>
       </c>
@@ -2634,7 +2634,7 @@
       </c>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>13</v>
       </c>
@@ -2652,7 +2652,7 @@
       </c>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
         <v>16</v>
       </c>
@@ -2670,7 +2670,7 @@
       </c>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>13</v>
       </c>
@@ -2688,7 +2688,7 @@
       </c>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
         <v>16</v>
       </c>
@@ -2706,7 +2706,7 @@
       </c>
       <c r="G27" s="7"/>
     </row>
-    <row r="28" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>13</v>
       </c>
@@ -2724,7 +2724,7 @@
       </c>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
         <v>16</v>
       </c>
@@ -2742,7 +2742,7 @@
       </c>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>13</v>
       </c>
@@ -2760,7 +2760,7 @@
       </c>
       <c r="G30" s="7"/>
     </row>
-    <row r="31" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
         <v>16</v>
       </c>
@@ -2777,7 +2777,7 @@
       <c r="G31" s="7"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
         <v>14</v>
       </c>
@@ -2795,7 +2795,7 @@
       </c>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
         <v>14</v>
       </c>
@@ -2811,7 +2811,7 @@
       </c>
       <c r="G33" s="7"/>
     </row>
-    <row r="34" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
         <v>14</v>
       </c>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>14</v>
       </c>
@@ -2847,7 +2847,7 @@
       </c>
       <c r="G35" s="7"/>
     </row>
-    <row r="36" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B36" s="8" t="s">
         <v>14</v>
       </c>
@@ -2865,7 +2865,7 @@
       </c>
       <c r="G36" s="7"/>
     </row>
-    <row r="37" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
         <v>14</v>
       </c>
@@ -2883,7 +2883,7 @@
       </c>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
         <v>14</v>
       </c>
@@ -2901,7 +2901,7 @@
       </c>
       <c r="G38" s="7"/>
     </row>
-    <row r="39" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B39" s="9" t="s">
         <v>15</v>
       </c>
@@ -2919,7 +2919,7 @@
       </c>
       <c r="G39" s="7"/>
     </row>
-    <row r="40" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B40" s="9" t="s">
         <v>15</v>
       </c>
@@ -2937,7 +2937,7 @@
       </c>
       <c r="G40" s="7"/>
     </row>
-    <row r="41" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B41" s="59" t="s">
         <v>36</v>
       </c>
@@ -2947,7 +2947,7 @@
       <c r="F41" s="60"/>
       <c r="G41" s="60"/>
     </row>
-    <row r="42" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B42" s="63"/>
       <c r="C42" s="64"/>
       <c r="D42" s="64"/>
@@ -2955,7 +2955,7 @@
       <c r="F42" s="64"/>
       <c r="G42" s="64"/>
     </row>
-    <row r="43" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>12</v>
       </c>
@@ -2973,7 +2973,7 @@
       </c>
       <c r="G43" s="7"/>
     </row>
-    <row r="44" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>13</v>
       </c>
@@ -2991,7 +2991,7 @@
       </c>
       <c r="G44" s="7"/>
     </row>
-    <row r="45" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>12</v>
       </c>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="G45" s="7"/>
     </row>
-    <row r="46" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>12</v>
       </c>
@@ -3027,7 +3027,7 @@
       </c>
       <c r="G46" s="7"/>
     </row>
-    <row r="47" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>12</v>
       </c>
@@ -3045,7 +3045,7 @@
       </c>
       <c r="G47" s="7"/>
     </row>
-    <row r="48" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B48" s="8" t="s">
         <v>14</v>
       </c>
@@ -3063,7 +3063,7 @@
       </c>
       <c r="G48" s="11"/>
     </row>
-    <row r="49" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B49" s="9" t="s">
         <v>15</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
         <v>15</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B51" s="9" t="s">
         <v>15</v>
       </c>
@@ -3148,7 +3148,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>9</v>
       </c>
@@ -3177,7 +3177,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
         <v>9</v>
       </c>
@@ -3206,7 +3206,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>9</v>
       </c>
@@ -3235,7 +3235,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B55" s="6" t="s">
         <v>13</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="56" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B56" s="6" t="s">
         <v>13</v>
       </c>
@@ -3280,7 +3280,7 @@
       </c>
       <c r="G56" s="11"/>
     </row>
-    <row r="57" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B57" s="10" t="s">
         <v>16</v>
       </c>
@@ -3298,7 +3298,7 @@
       </c>
       <c r="G57" s="7"/>
     </row>
-    <row r="58" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B58" s="10" t="s">
         <v>16</v>
       </c>
@@ -3325,7 +3325,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B59" s="10" t="s">
         <v>16</v>
       </c>
@@ -3354,7 +3354,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="60" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B60" s="10" t="s">
         <v>16</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B61" s="6" t="s">
         <v>13</v>
       </c>
@@ -3901,7 +3901,7 @@
       <c r="F84" s="34"/>
       <c r="G84" s="34"/>
     </row>
-    <row r="85" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B85" s="8" t="s">
         <v>14</v>
       </c>
@@ -4055,7 +4055,7 @@
       </c>
       <c r="G93" s="7"/>
     </row>
-    <row r="94" spans="2:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:7" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="4" t="s">
         <v>9</v>
       </c>
@@ -4744,13 +4744,13 @@
       <c r="F133" s="13">
         <v>6.5</v>
       </c>
-      <c r="G133" s="13"/>
+      <c r="G133" s="11"/>
       <c r="I133" s="5" t="s">
         <v>12</v>
       </c>
       <c r="J133">
         <f>F134</f>
-        <v>12.5</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="K133">
         <f>E134</f>
@@ -4769,15 +4769,19 @@
         <v>6</v>
       </c>
       <c r="F134" s="13">
-        <v>12.5</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="G134" s="11"/>
       <c r="I134" s="8" t="s">
         <v>14</v>
       </c>
       <c r="J134">
-        <f>E135 + E136</f>
-        <v>16</v>
+        <f>F136 + F135</f>
+        <v>18</v>
+      </c>
+      <c r="K134">
+        <f>E135+E136</f>
+        <v>8</v>
       </c>
     </row>
     <row r="135" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4789,10 +4793,12 @@
       </c>
       <c r="D135" s="13"/>
       <c r="E135" s="13">
+        <v>8</v>
+      </c>
+      <c r="F135" s="13">
         <v>16</v>
       </c>
-      <c r="F135" s="13"/>
-      <c r="G135" s="13"/>
+      <c r="G135" s="11"/>
       <c r="I135" s="10" t="s">
         <v>16</v>
       </c>
@@ -4810,8 +4816,10 @@
       </c>
       <c r="D136" s="13"/>
       <c r="E136" s="13"/>
-      <c r="F136" s="13"/>
-      <c r="G136" s="13"/>
+      <c r="F136" s="13">
+        <v>2</v>
+      </c>
+      <c r="G136" s="11"/>
     </row>
     <row r="137" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B137" s="54" t="s">
@@ -4938,13 +4946,13 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.54296875" customWidth="1"/>
-    <col min="2" max="2" width="35.453125" customWidth="1"/>
-    <col min="3" max="3" width="27.36328125" customWidth="1"/>
-    <col min="4" max="4" width="10.36328125" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5007,7 +5015,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -5030,7 +5038,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -5272,7 +5280,7 @@
       <c r="F17" s="13"/>
       <c r="G17" s="15"/>
     </row>
-    <row r="18" spans="1:7" ht="14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>17</v>
       </c>
@@ -5295,7 +5303,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>18</v>
       </c>
@@ -5318,7 +5326,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>19</v>
       </c>
@@ -5332,7 +5340,7 @@
       <c r="F20" s="13"/>
       <c r="G20" s="15"/>
     </row>
-    <row r="21" spans="1:7" ht="14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>20</v>
       </c>
@@ -5353,7 +5361,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>21</v>
       </c>
@@ -5368,7 +5376,7 @@
       <c r="F22" s="13"/>
       <c r="G22" s="15"/>
     </row>
-    <row r="23" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>22</v>
       </c>
@@ -5383,7 +5391,7 @@
       <c r="F23" s="13"/>
       <c r="G23" s="15"/>
     </row>
-    <row r="24" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>23</v>
       </c>
@@ -5404,7 +5412,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>24</v>
       </c>
@@ -5419,7 +5427,7 @@
       <c r="F25" s="13"/>
       <c r="G25" s="15"/>
     </row>
-    <row r="26" spans="1:7" ht="14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>25</v>
       </c>
@@ -5442,7 +5450,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>26</v>
       </c>
@@ -5457,7 +5465,7 @@
       <c r="F27" s="13"/>
       <c r="G27" s="15"/>
     </row>
-    <row r="28" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>27</v>
       </c>
@@ -5480,7 +5488,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>28</v>
       </c>
@@ -5495,7 +5503,7 @@
       <c r="F29" s="13"/>
       <c r="G29" s="15"/>
     </row>
-    <row r="30" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>29</v>
       </c>
@@ -5510,7 +5518,7 @@
       <c r="F30" s="13"/>
       <c r="G30" s="15"/>
     </row>
-    <row r="31" spans="1:7" ht="14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <v>30</v>
       </c>
@@ -5533,7 +5541,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <v>31</v>
       </c>
@@ -5554,7 +5562,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <v>32</v>
       </c>
@@ -5575,7 +5583,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <v>33</v>
       </c>
@@ -5596,7 +5604,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>34</v>
       </c>
@@ -5613,7 +5621,7 @@
       <c r="F35" s="13"/>
       <c r="G35" s="15"/>
     </row>
-    <row r="36" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>35</v>
       </c>
@@ -5628,7 +5636,7 @@
       <c r="F36" s="13"/>
       <c r="G36" s="15"/>
     </row>
-    <row r="37" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>36</v>
       </c>
@@ -5651,7 +5659,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <v>37</v>
       </c>
@@ -5668,7 +5676,7 @@
       <c r="F38" s="13"/>
       <c r="G38" s="15"/>
     </row>
-    <row r="39" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <v>38</v>
       </c>
@@ -5683,7 +5691,7 @@
       <c r="F39" s="13"/>
       <c r="G39" s="15"/>
     </row>
-    <row r="40" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <v>39</v>
       </c>
@@ -5704,7 +5712,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <v>40</v>
       </c>
@@ -5727,7 +5735,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <v>41</v>
       </c>
@@ -5750,7 +5758,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <v>42</v>
       </c>
@@ -5773,7 +5781,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <v>43</v>
       </c>
@@ -5796,7 +5804,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <v>44</v>
       </c>
@@ -5817,7 +5825,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <v>45</v>
       </c>
@@ -5832,7 +5840,7 @@
       <c r="F46" s="13"/>
       <c r="G46" s="15"/>
     </row>
-    <row r="47" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <v>46</v>
       </c>
@@ -5902,23 +5910,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002ACE3BD3BD6E0C4C9762278BB0DF607B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fab7ba1af23be20b30c2a2672ed67a22">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf" xmlns:ns4="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="531abb56a789977dee09b3cb67363cc8" ns3:_="" ns4:_="">
     <xsd:import namespace="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
@@ -6127,10 +6118,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6153,20 +6172,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
FInalizada la ruleta rusa. Ya nos podemos pegar tiros :) + Excel
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 4ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 4ª Version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2E1F8D-FDB3-467E-8F13-151B2AFC0C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF444C5-979B-4218-BC32-44BC05E0C0C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1014,7 +1014,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1167,7 +1167,6 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2188,8 +2187,8 @@
   </sheetPr>
   <dimension ref="A2:P150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="60" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E147" sqref="E147"/>
+    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="60" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G98" sqref="G98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2239,11 +2238,11 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1">
         <f t="shared" ref="E3:F3" si="0">SUM(E6:E996)</f>
-        <v>298.2</v>
+        <v>300.2</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>401.36</v>
+        <v>404.11</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
@@ -2298,8 +2297,8 @@
         <v>12</v>
       </c>
       <c r="K6" s="69">
-        <f>F7+F13+F20+F43+F45+F47+F46+J76+J133</f>
-        <v>64.5</v>
+        <f>F7+F13+F20+F43+F45+F47+F46+J76+J133+J148</f>
+        <v>67.25</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -4158,7 +4157,7 @@
       </c>
       <c r="E98" s="37"/>
       <c r="F98" s="37"/>
-      <c r="G98" s="11"/>
+      <c r="G98" s="7"/>
     </row>
     <row r="99" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" s="5" t="s">
@@ -4176,7 +4175,7 @@
       <c r="F99" s="37">
         <v>5</v>
       </c>
-      <c r="G99" s="11"/>
+      <c r="G99" s="7"/>
     </row>
     <row r="100" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B100" s="5" t="s">
@@ -4448,7 +4447,7 @@
       <c r="F115" s="37">
         <v>6</v>
       </c>
-      <c r="G115" s="11"/>
+      <c r="G115" s="7"/>
     </row>
     <row r="116" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="5" t="s">
@@ -4790,7 +4789,7 @@
       <c r="F134" s="13">
         <v>17.399999999999999</v>
       </c>
-      <c r="G134" s="11"/>
+      <c r="G134" s="7"/>
       <c r="I134" s="8" t="s">
         <v>14</v>
       </c>
@@ -4950,13 +4949,17 @@
       <c r="B144" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="C144" s="82" t="s">
+      <c r="C144" s="13" t="s">
         <v>189</v>
       </c>
       <c r="D144" s="13"/>
-      <c r="E144" s="13"/>
-      <c r="F144" s="13"/>
-      <c r="G144" s="13"/>
+      <c r="E144" s="13">
+        <v>2</v>
+      </c>
+      <c r="F144" s="13">
+        <v>2.75</v>
+      </c>
+      <c r="G144" s="7"/>
       <c r="I144" s="58" t="s">
         <v>188</v>
       </c>
@@ -4967,11 +4970,11 @@
         <v>46</v>
       </c>
     </row>
-    <row r="145" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B145" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="C145" s="82" t="s">
+      <c r="C145" s="13" t="s">
         <v>190</v>
       </c>
       <c r="D145" s="13"/>
@@ -4982,11 +4985,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B146" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="C146" s="82" t="s">
+      <c r="C146" s="13" t="s">
         <v>191</v>
       </c>
       <c r="D146" s="13"/>
@@ -4997,11 +5000,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="147" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B147" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="C147" s="82" t="s">
+      <c r="C147" s="13" t="s">
         <v>192</v>
       </c>
       <c r="D147" s="13"/>
@@ -5012,23 +5015,32 @@
         <v>15</v>
       </c>
     </row>
-    <row r="148" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I148" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="149" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J148">
+        <f>F144</f>
+        <v>2.75</v>
+      </c>
+      <c r="K148">
+        <f>E144</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I149" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="150" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I150" s="10" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="J22:L22"/>
     <mergeCell ref="B142:G143"/>
     <mergeCell ref="B127:G128"/>
     <mergeCell ref="B72:G73"/>
@@ -5045,7 +5057,6 @@
     <mergeCell ref="K18:K20"/>
     <mergeCell ref="J18:J20"/>
     <mergeCell ref="B4:G5"/>
-    <mergeCell ref="J22:L22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6029,23 +6040,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002ACE3BD3BD6E0C4C9762278BB0DF607B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fab7ba1af23be20b30c2a2672ed67a22">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf" xmlns:ns4="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="531abb56a789977dee09b3cb67363cc8" ns3:_="" ns4:_="">
     <xsd:import namespace="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
@@ -6254,10 +6248,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6280,20 +6302,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>